<commit_message>
Atualizado bug no somatório do modelo mdiario_adm.xlsx
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IEI.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IEI.XLSX
@@ -1983,263 +1983,113 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -2249,135 +2099,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2429,16 +2150,295 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2748,7 +2748,7 @@
   <dimension ref="A1:BH56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="M13" sqref="M13:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2767,78 +2767,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="177" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="96" t="s">
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="179"/>
+      <c r="F1" s="183" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="132" t="s">
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
+      <c r="J1" s="184"/>
+      <c r="K1" s="184"/>
+      <c r="L1" s="185"/>
+      <c r="M1" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="133"/>
-      <c r="O1" s="133"/>
-      <c r="P1" s="133"/>
-      <c r="Q1" s="133"/>
-      <c r="R1" s="133"/>
-      <c r="S1" s="133"/>
-      <c r="T1" s="134"/>
+      <c r="N1" s="187"/>
+      <c r="O1" s="187"/>
+      <c r="P1" s="187"/>
+      <c r="Q1" s="187"/>
+      <c r="R1" s="187"/>
+      <c r="S1" s="187"/>
+      <c r="T1" s="188"/>
       <c r="U1" s="6"/>
-      <c r="V1" s="122" t="s">
+      <c r="V1" s="225" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="122"/>
-      <c r="X1" s="122"/>
-      <c r="Y1" s="122"/>
-      <c r="Z1" s="122"/>
-      <c r="AA1" s="122"/>
-      <c r="AB1" s="123"/>
-      <c r="AC1" s="107" t="s">
+      <c r="W1" s="225"/>
+      <c r="X1" s="225"/>
+      <c r="Y1" s="225"/>
+      <c r="Z1" s="225"/>
+      <c r="AA1" s="225"/>
+      <c r="AB1" s="226"/>
+      <c r="AC1" s="210" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="108"/>
-      <c r="AF1" s="108"/>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="108"/>
-      <c r="AI1" s="108"/>
-      <c r="AJ1" s="108"/>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
-      <c r="AN1" s="109"/>
+      <c r="AD1" s="144"/>
+      <c r="AE1" s="144"/>
+      <c r="AF1" s="144"/>
+      <c r="AG1" s="144"/>
+      <c r="AH1" s="144"/>
+      <c r="AI1" s="144"/>
+      <c r="AJ1" s="144"/>
+      <c r="AK1" s="144"/>
+      <c r="AL1" s="144"/>
+      <c r="AM1" s="144"/>
+      <c r="AN1" s="211"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="128"/>
-      <c r="B2" s="129"/>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="118"/>
+      <c r="A2" s="180"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="214"/>
+      <c r="G2" s="215"/>
+      <c r="H2" s="215"/>
+      <c r="I2" s="215"/>
+      <c r="J2" s="215"/>
+      <c r="K2" s="215"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="217"/>
+      <c r="N2" s="218"/>
+      <c r="O2" s="218"/>
+      <c r="P2" s="218"/>
+      <c r="Q2" s="218"/>
+      <c r="R2" s="218"/>
+      <c r="S2" s="218"/>
+      <c r="T2" s="219"/>
       <c r="U2" s="7"/>
       <c r="V2" s="33"/>
       <c r="W2" s="33"/>
@@ -2847,25 +2847,25 @@
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
       <c r="AB2" s="34"/>
-      <c r="AC2" s="110"/>
-      <c r="AD2" s="111"/>
-      <c r="AE2" s="111"/>
-      <c r="AF2" s="111"/>
-      <c r="AG2" s="111"/>
-      <c r="AH2" s="111"/>
-      <c r="AI2" s="111"/>
-      <c r="AJ2" s="111"/>
-      <c r="AK2" s="111"/>
-      <c r="AL2" s="111"/>
-      <c r="AM2" s="111"/>
-      <c r="AN2" s="112"/>
+      <c r="AC2" s="212"/>
+      <c r="AD2" s="147"/>
+      <c r="AE2" s="147"/>
+      <c r="AF2" s="147"/>
+      <c r="AG2" s="147"/>
+      <c r="AH2" s="147"/>
+      <c r="AI2" s="147"/>
+      <c r="AJ2" s="147"/>
+      <c r="AK2" s="147"/>
+      <c r="AL2" s="147"/>
+      <c r="AM2" s="147"/>
+      <c r="AN2" s="213"/>
     </row>
     <row r="3" spans="1:40" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="128"/>
-      <c r="B3" s="129"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="130"/>
+      <c r="A3" s="180"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="182"/>
       <c r="F3" s="44"/>
       <c r="G3" s="45"/>
       <c r="H3" s="45"/>
@@ -2889,71 +2889,71 @@
       <c r="Z3" s="28"/>
       <c r="AA3" s="28"/>
       <c r="AB3" s="36"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="111"/>
-      <c r="AE3" s="111"/>
-      <c r="AF3" s="111"/>
-      <c r="AG3" s="111"/>
-      <c r="AH3" s="111"/>
-      <c r="AI3" s="111"/>
-      <c r="AJ3" s="111"/>
-      <c r="AK3" s="111"/>
-      <c r="AL3" s="111"/>
-      <c r="AM3" s="111"/>
-      <c r="AN3" s="112"/>
+      <c r="AC3" s="212"/>
+      <c r="AD3" s="147"/>
+      <c r="AE3" s="147"/>
+      <c r="AF3" s="147"/>
+      <c r="AG3" s="147"/>
+      <c r="AH3" s="147"/>
+      <c r="AI3" s="147"/>
+      <c r="AJ3" s="147"/>
+      <c r="AK3" s="147"/>
+      <c r="AL3" s="147"/>
+      <c r="AM3" s="147"/>
+      <c r="AN3" s="213"/>
     </row>
     <row r="4" spans="1:40" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="128"/>
-      <c r="B4" s="129"/>
-      <c r="C4" s="129"/>
-      <c r="D4" s="129"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="119" t="s">
+      <c r="A4" s="180"/>
+      <c r="B4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="222" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="120"/>
-      <c r="J4" s="120"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="121"/>
+      <c r="G4" s="223"/>
+      <c r="H4" s="223"/>
+      <c r="I4" s="223"/>
+      <c r="J4" s="223"/>
+      <c r="K4" s="223"/>
+      <c r="L4" s="224"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="233"/>
-      <c r="O4" s="233"/>
-      <c r="P4" s="233"/>
-      <c r="Q4" s="233"/>
-      <c r="R4" s="233"/>
-      <c r="S4" s="233"/>
+      <c r="N4" s="220"/>
+      <c r="O4" s="220"/>
+      <c r="P4" s="220"/>
+      <c r="Q4" s="220"/>
+      <c r="R4" s="220"/>
+      <c r="S4" s="220"/>
       <c r="T4" s="9"/>
       <c r="U4" s="24"/>
       <c r="V4" s="5"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="102" t="s">
+      <c r="X4" s="221" t="s">
         <v>13</v>
       </c>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="102"/>
-      <c r="AA4" s="102"/>
+      <c r="Y4" s="221"/>
+      <c r="Z4" s="221"/>
+      <c r="AA4" s="221"/>
       <c r="AB4" s="36"/>
-      <c r="AC4" s="110"/>
-      <c r="AD4" s="111"/>
-      <c r="AE4" s="111"/>
-      <c r="AF4" s="111"/>
-      <c r="AG4" s="111"/>
-      <c r="AH4" s="111"/>
-      <c r="AI4" s="111"/>
-      <c r="AJ4" s="111"/>
-      <c r="AK4" s="111"/>
-      <c r="AL4" s="111"/>
-      <c r="AM4" s="111"/>
-      <c r="AN4" s="112"/>
+      <c r="AC4" s="212"/>
+      <c r="AD4" s="147"/>
+      <c r="AE4" s="147"/>
+      <c r="AF4" s="147"/>
+      <c r="AG4" s="147"/>
+      <c r="AH4" s="147"/>
+      <c r="AI4" s="147"/>
+      <c r="AJ4" s="147"/>
+      <c r="AK4" s="147"/>
+      <c r="AL4" s="147"/>
+      <c r="AM4" s="147"/>
+      <c r="AN4" s="213"/>
     </row>
     <row r="5" spans="1:40" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="128"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="130"/>
+      <c r="A5" s="180"/>
+      <c r="B5" s="181"/>
+      <c r="C5" s="181"/>
+      <c r="D5" s="181"/>
+      <c r="E5" s="182"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2962,12 +2962,12 @@
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
       <c r="M5" s="8"/>
-      <c r="N5" s="231"/>
-      <c r="O5" s="231"/>
-      <c r="P5" s="231"/>
-      <c r="Q5" s="231"/>
-      <c r="R5" s="232"/>
-      <c r="S5" s="232"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="88"/>
+      <c r="S5" s="88"/>
       <c r="T5" s="9"/>
       <c r="U5" s="24"/>
       <c r="V5" s="1"/>
@@ -2977,73 +2977,73 @@
       <c r="Z5" s="23"/>
       <c r="AA5" s="23"/>
       <c r="AB5" s="37"/>
-      <c r="AC5" s="96" t="s">
+      <c r="AC5" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="AD5" s="97"/>
-      <c r="AE5" s="97"/>
-      <c r="AF5" s="97"/>
-      <c r="AG5" s="97"/>
-      <c r="AH5" s="97"/>
-      <c r="AI5" s="97"/>
-      <c r="AJ5" s="97"/>
-      <c r="AK5" s="97"/>
-      <c r="AL5" s="97"/>
-      <c r="AM5" s="97"/>
-      <c r="AN5" s="98"/>
+      <c r="AD5" s="184"/>
+      <c r="AE5" s="184"/>
+      <c r="AF5" s="184"/>
+      <c r="AG5" s="184"/>
+      <c r="AH5" s="184"/>
+      <c r="AI5" s="184"/>
+      <c r="AJ5" s="184"/>
+      <c r="AK5" s="184"/>
+      <c r="AL5" s="184"/>
+      <c r="AM5" s="184"/>
+      <c r="AN5" s="228"/>
     </row>
     <row r="6" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="128"/>
-      <c r="B6" s="129"/>
-      <c r="C6" s="129"/>
-      <c r="D6" s="129"/>
-      <c r="E6" s="130"/>
-      <c r="F6" s="99" t="s">
+      <c r="A6" s="180"/>
+      <c r="B6" s="181"/>
+      <c r="C6" s="181"/>
+      <c r="D6" s="181"/>
+      <c r="E6" s="182"/>
+      <c r="F6" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="124"/>
+      <c r="G6" s="175"/>
+      <c r="H6" s="175"/>
+      <c r="I6" s="175"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="175"/>
+      <c r="L6" s="176"/>
       <c r="M6" s="8"/>
-      <c r="N6" s="231"/>
-      <c r="O6" s="231"/>
-      <c r="P6" s="231"/>
-      <c r="Q6" s="231"/>
-      <c r="R6" s="231"/>
-      <c r="S6" s="231"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
       <c r="T6" s="9"/>
       <c r="U6" s="7"/>
       <c r="V6" s="5"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="102" t="s">
+      <c r="X6" s="221" t="s">
         <v>15</v>
       </c>
-      <c r="Y6" s="102"/>
-      <c r="Z6" s="102"/>
-      <c r="AA6" s="102"/>
-      <c r="AB6" s="103"/>
-      <c r="AC6" s="99"/>
-      <c r="AD6" s="100"/>
-      <c r="AE6" s="100"/>
-      <c r="AF6" s="100"/>
-      <c r="AG6" s="100"/>
-      <c r="AH6" s="100"/>
-      <c r="AI6" s="100"/>
-      <c r="AJ6" s="100"/>
-      <c r="AK6" s="100"/>
-      <c r="AL6" s="100"/>
-      <c r="AM6" s="100"/>
-      <c r="AN6" s="101"/>
+      <c r="Y6" s="221"/>
+      <c r="Z6" s="221"/>
+      <c r="AA6" s="221"/>
+      <c r="AB6" s="230"/>
+      <c r="AC6" s="174"/>
+      <c r="AD6" s="175"/>
+      <c r="AE6" s="175"/>
+      <c r="AF6" s="175"/>
+      <c r="AG6" s="175"/>
+      <c r="AH6" s="175"/>
+      <c r="AI6" s="175"/>
+      <c r="AJ6" s="175"/>
+      <c r="AK6" s="175"/>
+      <c r="AL6" s="175"/>
+      <c r="AM6" s="175"/>
+      <c r="AN6" s="229"/>
     </row>
     <row r="7" spans="1:40" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="128"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="130"/>
+      <c r="A7" s="180"/>
+      <c r="B7" s="181"/>
+      <c r="C7" s="181"/>
+      <c r="D7" s="181"/>
+      <c r="E7" s="182"/>
       <c r="F7" s="41"/>
       <c r="G7" s="42"/>
       <c r="H7" s="42"/>
@@ -3052,12 +3052,12 @@
       <c r="K7" s="42"/>
       <c r="L7" s="43"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="104"/>
-      <c r="O7" s="105"/>
-      <c r="P7" s="106"/>
-      <c r="Q7" s="105"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="104"/>
+      <c r="N7" s="231"/>
+      <c r="O7" s="232"/>
+      <c r="P7" s="233"/>
+      <c r="Q7" s="232"/>
+      <c r="R7" s="233"/>
+      <c r="S7" s="231"/>
       <c r="T7" s="11"/>
       <c r="U7" s="7"/>
       <c r="V7" s="1"/>
@@ -3067,34 +3067,34 @@
       <c r="Z7" s="23"/>
       <c r="AA7" s="23"/>
       <c r="AB7" s="37"/>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="100"/>
-      <c r="AE7" s="100"/>
-      <c r="AF7" s="100"/>
-      <c r="AG7" s="100"/>
-      <c r="AH7" s="100"/>
-      <c r="AI7" s="100"/>
-      <c r="AJ7" s="100"/>
-      <c r="AK7" s="100"/>
-      <c r="AL7" s="100"/>
-      <c r="AM7" s="100"/>
-      <c r="AN7" s="101"/>
+      <c r="AC7" s="174"/>
+      <c r="AD7" s="175"/>
+      <c r="AE7" s="175"/>
+      <c r="AF7" s="175"/>
+      <c r="AG7" s="175"/>
+      <c r="AH7" s="175"/>
+      <c r="AI7" s="175"/>
+      <c r="AJ7" s="175"/>
+      <c r="AK7" s="175"/>
+      <c r="AL7" s="175"/>
+      <c r="AM7" s="175"/>
+      <c r="AN7" s="229"/>
     </row>
     <row r="8" spans="1:40" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="128"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="129"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="99" t="s">
+      <c r="A8" s="180"/>
+      <c r="B8" s="181"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="174" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="100"/>
-      <c r="H8" s="100"/>
-      <c r="I8" s="100"/>
-      <c r="J8" s="100"/>
-      <c r="K8" s="100"/>
-      <c r="L8" s="124"/>
+      <c r="G8" s="175"/>
+      <c r="H8" s="175"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="175"/>
+      <c r="K8" s="175"/>
+      <c r="L8" s="176"/>
       <c r="M8" s="12"/>
       <c r="N8" s="13"/>
       <c r="O8" s="14"/>
@@ -3106,82 +3106,82 @@
       <c r="U8" s="7"/>
       <c r="V8" s="5"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="102" t="s">
+      <c r="X8" s="221" t="s">
         <v>14</v>
       </c>
-      <c r="Y8" s="102"/>
-      <c r="Z8" s="102"/>
-      <c r="AA8" s="102"/>
-      <c r="AB8" s="103"/>
-      <c r="AC8" s="99"/>
-      <c r="AD8" s="100"/>
-      <c r="AE8" s="100"/>
-      <c r="AF8" s="100"/>
-      <c r="AG8" s="100"/>
-      <c r="AH8" s="100"/>
-      <c r="AI8" s="100"/>
-      <c r="AJ8" s="100"/>
-      <c r="AK8" s="100"/>
-      <c r="AL8" s="100"/>
-      <c r="AM8" s="100"/>
-      <c r="AN8" s="101"/>
+      <c r="Y8" s="221"/>
+      <c r="Z8" s="221"/>
+      <c r="AA8" s="221"/>
+      <c r="AB8" s="230"/>
+      <c r="AC8" s="174"/>
+      <c r="AD8" s="175"/>
+      <c r="AE8" s="175"/>
+      <c r="AF8" s="175"/>
+      <c r="AG8" s="175"/>
+      <c r="AH8" s="175"/>
+      <c r="AI8" s="175"/>
+      <c r="AJ8" s="175"/>
+      <c r="AK8" s="175"/>
+      <c r="AL8" s="175"/>
+      <c r="AM8" s="175"/>
+      <c r="AN8" s="229"/>
     </row>
     <row r="9" spans="1:40" ht="4.9000000000000004" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="128"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="129"/>
-      <c r="E9" s="130"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="100"/>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="140"/>
-      <c r="N9" s="141"/>
-      <c r="O9" s="141"/>
-      <c r="P9" s="141"/>
-      <c r="Q9" s="141"/>
-      <c r="R9" s="141"/>
-      <c r="S9" s="141"/>
-      <c r="T9" s="142"/>
+      <c r="A9" s="180"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="182"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="175"/>
+      <c r="H9" s="175"/>
+      <c r="I9" s="175"/>
+      <c r="J9" s="175"/>
+      <c r="K9" s="175"/>
+      <c r="L9" s="176"/>
+      <c r="M9" s="192"/>
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193"/>
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="193"/>
+      <c r="T9" s="194"/>
       <c r="U9" s="24"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
-      <c r="X9" s="102"/>
-      <c r="Y9" s="102"/>
-      <c r="Z9" s="102"/>
-      <c r="AA9" s="102"/>
+      <c r="X9" s="221"/>
+      <c r="Y9" s="221"/>
+      <c r="Z9" s="221"/>
+      <c r="AA9" s="221"/>
       <c r="AB9" s="37"/>
-      <c r="AC9" s="99"/>
-      <c r="AD9" s="100"/>
-      <c r="AE9" s="100"/>
-      <c r="AF9" s="100"/>
-      <c r="AG9" s="100"/>
-      <c r="AH9" s="100"/>
-      <c r="AI9" s="100"/>
-      <c r="AJ9" s="100"/>
-      <c r="AK9" s="100"/>
-      <c r="AL9" s="100"/>
-      <c r="AM9" s="100"/>
-      <c r="AN9" s="101"/>
+      <c r="AC9" s="174"/>
+      <c r="AD9" s="175"/>
+      <c r="AE9" s="175"/>
+      <c r="AF9" s="175"/>
+      <c r="AG9" s="175"/>
+      <c r="AH9" s="175"/>
+      <c r="AI9" s="175"/>
+      <c r="AJ9" s="175"/>
+      <c r="AK9" s="175"/>
+      <c r="AL9" s="175"/>
+      <c r="AM9" s="175"/>
+      <c r="AN9" s="229"/>
     </row>
     <row r="10" spans="1:40" s="40" customFormat="1" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="151" t="s">
+      <c r="A10" s="201" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="137" t="s">
+      <c r="B10" s="189" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="154" t="s">
+      <c r="C10" s="204" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="157" t="s">
+      <c r="D10" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="157" t="s">
+      <c r="E10" s="207" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -3205,10 +3205,10 @@
       <c r="L10" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="M10" s="92" t="s">
+      <c r="M10" s="195" t="s">
         <v>67</v>
       </c>
-      <c r="N10" s="94"/>
+      <c r="N10" s="196"/>
       <c r="O10" s="49" t="s">
         <v>68</v>
       </c>
@@ -3221,15 +3221,15 @@
       <c r="R10" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="S10" s="92" t="s">
+      <c r="S10" s="195" t="s">
         <v>72</v>
       </c>
-      <c r="T10" s="94"/>
-      <c r="U10" s="92" t="s">
+      <c r="T10" s="196"/>
+      <c r="U10" s="195" t="s">
         <v>73</v>
       </c>
-      <c r="V10" s="93"/>
-      <c r="W10" s="94"/>
+      <c r="V10" s="227"/>
+      <c r="W10" s="196"/>
       <c r="X10" s="49" t="s">
         <v>74</v>
       </c>
@@ -3283,153 +3283,153 @@
       </c>
     </row>
     <row r="11" spans="1:40" ht="13.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="152"/>
-      <c r="B11" s="138"/>
-      <c r="C11" s="155"/>
-      <c r="D11" s="158"/>
-      <c r="E11" s="158"/>
-      <c r="F11" s="147" t="s">
+      <c r="A11" s="202"/>
+      <c r="B11" s="190"/>
+      <c r="C11" s="205"/>
+      <c r="D11" s="208"/>
+      <c r="E11" s="208"/>
+      <c r="F11" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="149" t="s">
+      <c r="G11" s="199" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="135" t="s">
+      <c r="H11" s="91" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="135" t="s">
+      <c r="I11" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="135" t="s">
+      <c r="J11" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="135" t="s">
+      <c r="K11" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="135" t="s">
+      <c r="L11" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="143" t="s">
+      <c r="M11" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="144"/>
-      <c r="O11" s="135" t="s">
+      <c r="N11" s="169"/>
+      <c r="O11" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="P11" s="135" t="s">
+      <c r="P11" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="135" t="s">
+      <c r="Q11" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="R11" s="135" t="s">
+      <c r="R11" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="S11" s="143" t="s">
+      <c r="S11" s="168" t="s">
         <v>44</v>
       </c>
-      <c r="T11" s="144"/>
-      <c r="U11" s="143" t="s">
+      <c r="T11" s="169"/>
+      <c r="U11" s="168" t="s">
         <v>45</v>
       </c>
-      <c r="V11" s="160"/>
-      <c r="W11" s="144"/>
-      <c r="X11" s="135" t="s">
+      <c r="V11" s="172"/>
+      <c r="W11" s="169"/>
+      <c r="X11" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="Y11" s="135" t="s">
+      <c r="Y11" s="91" t="s">
         <v>47</v>
       </c>
-      <c r="Z11" s="135" t="s">
+      <c r="Z11" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="AA11" s="135" t="s">
+      <c r="AA11" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="AB11" s="135" t="s">
+      <c r="AB11" s="91" t="s">
         <v>50</v>
       </c>
-      <c r="AC11" s="135" t="s">
+      <c r="AC11" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="AD11" s="135" t="s">
+      <c r="AD11" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="AE11" s="135" t="s">
+      <c r="AE11" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="AF11" s="135" t="s">
+      <c r="AF11" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="AG11" s="135" t="s">
+      <c r="AG11" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="AH11" s="135" t="s">
+      <c r="AH11" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="AI11" s="135" t="s">
+      <c r="AI11" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="AJ11" s="135" t="s">
+      <c r="AJ11" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="AK11" s="135" t="s">
+      <c r="AK11" s="91" t="s">
         <v>59</v>
       </c>
-      <c r="AL11" s="135" t="s">
+      <c r="AL11" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="AM11" s="135" t="s">
+      <c r="AM11" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="AN11" s="162" t="s">
+      <c r="AN11" s="160" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="153"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="156"/>
-      <c r="D12" s="159"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="148"/>
-      <c r="G12" s="150"/>
-      <c r="H12" s="136"/>
-      <c r="I12" s="136"/>
-      <c r="J12" s="136"/>
-      <c r="K12" s="136"/>
-      <c r="L12" s="136"/>
-      <c r="M12" s="145"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="136"/>
-      <c r="P12" s="136"/>
-      <c r="Q12" s="136"/>
-      <c r="R12" s="136"/>
-      <c r="S12" s="145"/>
-      <c r="T12" s="146"/>
-      <c r="U12" s="145"/>
-      <c r="V12" s="161"/>
-      <c r="W12" s="146"/>
-      <c r="X12" s="136"/>
-      <c r="Y12" s="136"/>
-      <c r="Z12" s="136"/>
-      <c r="AA12" s="136"/>
-      <c r="AB12" s="136"/>
-      <c r="AC12" s="136"/>
-      <c r="AD12" s="136"/>
-      <c r="AE12" s="136"/>
-      <c r="AF12" s="136"/>
-      <c r="AG12" s="136"/>
-      <c r="AH12" s="136"/>
-      <c r="AI12" s="136"/>
-      <c r="AJ12" s="136"/>
-      <c r="AK12" s="136"/>
-      <c r="AL12" s="136"/>
-      <c r="AM12" s="136"/>
-      <c r="AN12" s="163"/>
+      <c r="A12" s="203"/>
+      <c r="B12" s="191"/>
+      <c r="C12" s="206"/>
+      <c r="D12" s="209"/>
+      <c r="E12" s="209"/>
+      <c r="F12" s="198"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="170"/>
+      <c r="N12" s="171"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="92"/>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="92"/>
+      <c r="S12" s="170"/>
+      <c r="T12" s="171"/>
+      <c r="U12" s="170"/>
+      <c r="V12" s="173"/>
+      <c r="W12" s="171"/>
+      <c r="X12" s="92"/>
+      <c r="Y12" s="92"/>
+      <c r="Z12" s="92"/>
+      <c r="AA12" s="92"/>
+      <c r="AB12" s="92"/>
+      <c r="AC12" s="92"/>
+      <c r="AD12" s="92"/>
+      <c r="AE12" s="92"/>
+      <c r="AF12" s="92"/>
+      <c r="AG12" s="92"/>
+      <c r="AH12" s="92"/>
+      <c r="AI12" s="92"/>
+      <c r="AJ12" s="92"/>
+      <c r="AK12" s="92"/>
+      <c r="AL12" s="92"/>
+      <c r="AM12" s="92"/>
+      <c r="AN12" s="161"/>
     </row>
     <row r="13" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="164" t="s">
+      <c r="A13" s="162" t="s">
         <v>91</v>
       </c>
       <c r="B13" s="17"/>
@@ -3443,17 +3443,17 @@
       <c r="J13" s="55"/>
       <c r="K13" s="55"/>
       <c r="L13" s="55"/>
-      <c r="M13" s="167"/>
-      <c r="N13" s="168"/>
+      <c r="M13" s="165"/>
+      <c r="N13" s="166"/>
       <c r="O13" s="55"/>
       <c r="P13" s="55"/>
       <c r="Q13" s="55"/>
       <c r="R13" s="55"/>
-      <c r="S13" s="167"/>
-      <c r="T13" s="168"/>
-      <c r="U13" s="167"/>
-      <c r="V13" s="169"/>
-      <c r="W13" s="168"/>
+      <c r="S13" s="165"/>
+      <c r="T13" s="166"/>
+      <c r="U13" s="165"/>
+      <c r="V13" s="167"/>
+      <c r="W13" s="166"/>
       <c r="X13" s="55"/>
       <c r="Y13" s="55"/>
       <c r="Z13" s="55"/>
@@ -3473,7 +3473,7 @@
       <c r="AN13" s="58"/>
     </row>
     <row r="14" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="165"/>
+      <c r="A14" s="163"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
@@ -3485,17 +3485,17 @@
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
       <c r="L14" s="60"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="88"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="95"/>
       <c r="O14" s="60"/>
       <c r="P14" s="60"/>
       <c r="Q14" s="60"/>
       <c r="R14" s="60"/>
-      <c r="S14" s="87"/>
-      <c r="T14" s="88"/>
-      <c r="U14" s="87"/>
-      <c r="V14" s="89"/>
-      <c r="W14" s="88"/>
+      <c r="S14" s="96"/>
+      <c r="T14" s="95"/>
+      <c r="U14" s="96"/>
+      <c r="V14" s="97"/>
+      <c r="W14" s="95"/>
       <c r="X14" s="60"/>
       <c r="Y14" s="60"/>
       <c r="Z14" s="60"/>
@@ -3515,7 +3515,7 @@
       <c r="AN14" s="63"/>
     </row>
     <row r="15" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="165"/>
+      <c r="A15" s="163"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
@@ -3527,17 +3527,17 @@
       <c r="J15" s="65"/>
       <c r="K15" s="65"/>
       <c r="L15" s="65"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="91"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="90"/>
       <c r="O15" s="65"/>
       <c r="P15" s="65"/>
       <c r="Q15" s="65"/>
       <c r="R15" s="65"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="91"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="95"/>
-      <c r="W15" s="91"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="90"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="98"/>
+      <c r="W15" s="90"/>
       <c r="X15" s="65"/>
       <c r="Y15" s="65"/>
       <c r="Z15" s="65"/>
@@ -3557,7 +3557,7 @@
       <c r="AN15" s="68"/>
     </row>
     <row r="16" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="165"/>
+      <c r="A16" s="163"/>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
@@ -3569,17 +3569,17 @@
       <c r="J16" s="60"/>
       <c r="K16" s="60"/>
       <c r="L16" s="60"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="88"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="95"/>
       <c r="O16" s="60"/>
       <c r="P16" s="60"/>
       <c r="Q16" s="60"/>
       <c r="R16" s="60"/>
-      <c r="S16" s="87"/>
-      <c r="T16" s="88"/>
-      <c r="U16" s="87"/>
-      <c r="V16" s="89"/>
-      <c r="W16" s="88"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="95"/>
+      <c r="U16" s="96"/>
+      <c r="V16" s="97"/>
+      <c r="W16" s="95"/>
       <c r="X16" s="60"/>
       <c r="Y16" s="60"/>
       <c r="Z16" s="60"/>
@@ -3599,7 +3599,7 @@
       <c r="AN16" s="63"/>
     </row>
     <row r="17" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="165"/>
+      <c r="A17" s="163"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
@@ -3611,17 +3611,17 @@
       <c r="J17" s="65"/>
       <c r="K17" s="65"/>
       <c r="L17" s="65"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="91"/>
+      <c r="M17" s="89"/>
+      <c r="N17" s="90"/>
       <c r="O17" s="65"/>
       <c r="P17" s="65"/>
       <c r="Q17" s="65"/>
       <c r="R17" s="65"/>
-      <c r="S17" s="90"/>
-      <c r="T17" s="91"/>
-      <c r="U17" s="90"/>
-      <c r="V17" s="95"/>
-      <c r="W17" s="91"/>
+      <c r="S17" s="89"/>
+      <c r="T17" s="90"/>
+      <c r="U17" s="89"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="90"/>
       <c r="X17" s="65"/>
       <c r="Y17" s="65"/>
       <c r="Z17" s="65"/>
@@ -3641,7 +3641,7 @@
       <c r="AN17" s="68"/>
     </row>
     <row r="18" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="165"/>
+      <c r="A18" s="163"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -3653,17 +3653,17 @@
       <c r="J18" s="60"/>
       <c r="K18" s="60"/>
       <c r="L18" s="60"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="88"/>
+      <c r="M18" s="96"/>
+      <c r="N18" s="95"/>
       <c r="O18" s="60"/>
       <c r="P18" s="60"/>
       <c r="Q18" s="60"/>
       <c r="R18" s="60"/>
-      <c r="S18" s="87"/>
-      <c r="T18" s="88"/>
-      <c r="U18" s="87"/>
-      <c r="V18" s="89"/>
-      <c r="W18" s="88"/>
+      <c r="S18" s="96"/>
+      <c r="T18" s="95"/>
+      <c r="U18" s="96"/>
+      <c r="V18" s="97"/>
+      <c r="W18" s="95"/>
       <c r="X18" s="60"/>
       <c r="Y18" s="60"/>
       <c r="Z18" s="60"/>
@@ -3683,7 +3683,7 @@
       <c r="AN18" s="63"/>
     </row>
     <row r="19" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="165"/>
+      <c r="A19" s="163"/>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
@@ -3695,17 +3695,17 @@
       <c r="J19" s="65"/>
       <c r="K19" s="65"/>
       <c r="L19" s="65"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="91"/>
+      <c r="M19" s="89"/>
+      <c r="N19" s="90"/>
       <c r="O19" s="65"/>
       <c r="P19" s="65"/>
       <c r="Q19" s="65"/>
       <c r="R19" s="65"/>
-      <c r="S19" s="90"/>
-      <c r="T19" s="91"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="95"/>
-      <c r="W19" s="91"/>
+      <c r="S19" s="89"/>
+      <c r="T19" s="90"/>
+      <c r="U19" s="89"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="90"/>
       <c r="X19" s="65"/>
       <c r="Y19" s="65"/>
       <c r="Z19" s="65"/>
@@ -3725,7 +3725,7 @@
       <c r="AN19" s="68"/>
     </row>
     <row r="20" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="165"/>
+      <c r="A20" s="163"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
@@ -3737,17 +3737,17 @@
       <c r="J20" s="60"/>
       <c r="K20" s="60"/>
       <c r="L20" s="60"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="88"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="95"/>
       <c r="O20" s="60"/>
       <c r="P20" s="60"/>
       <c r="Q20" s="60"/>
       <c r="R20" s="60"/>
-      <c r="S20" s="87"/>
-      <c r="T20" s="88"/>
-      <c r="U20" s="87"/>
-      <c r="V20" s="89"/>
-      <c r="W20" s="88"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="96"/>
+      <c r="V20" s="97"/>
+      <c r="W20" s="95"/>
       <c r="X20" s="60"/>
       <c r="Y20" s="60"/>
       <c r="Z20" s="60"/>
@@ -3767,7 +3767,7 @@
       <c r="AN20" s="63"/>
     </row>
     <row r="21" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="165"/>
+      <c r="A21" s="163"/>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="22"/>
@@ -3779,17 +3779,17 @@
       <c r="J21" s="65"/>
       <c r="K21" s="65"/>
       <c r="L21" s="65"/>
-      <c r="M21" s="90"/>
-      <c r="N21" s="91"/>
+      <c r="M21" s="89"/>
+      <c r="N21" s="90"/>
       <c r="O21" s="65"/>
       <c r="P21" s="65"/>
       <c r="Q21" s="65"/>
       <c r="R21" s="65"/>
-      <c r="S21" s="90"/>
-      <c r="T21" s="91"/>
-      <c r="U21" s="90"/>
-      <c r="V21" s="95"/>
-      <c r="W21" s="91"/>
+      <c r="S21" s="89"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="89"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="90"/>
       <c r="X21" s="65"/>
       <c r="Y21" s="65"/>
       <c r="Z21" s="65"/>
@@ -3809,7 +3809,7 @@
       <c r="AN21" s="68"/>
     </row>
     <row r="22" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="165"/>
+      <c r="A22" s="163"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
@@ -3821,17 +3821,17 @@
       <c r="J22" s="60"/>
       <c r="K22" s="60"/>
       <c r="L22" s="60"/>
-      <c r="M22" s="87"/>
-      <c r="N22" s="88"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="95"/>
       <c r="O22" s="60"/>
       <c r="P22" s="60"/>
       <c r="Q22" s="60"/>
       <c r="R22" s="60"/>
-      <c r="S22" s="87"/>
-      <c r="T22" s="88"/>
-      <c r="U22" s="87"/>
-      <c r="V22" s="89"/>
-      <c r="W22" s="88"/>
+      <c r="S22" s="96"/>
+      <c r="T22" s="95"/>
+      <c r="U22" s="96"/>
+      <c r="V22" s="97"/>
+      <c r="W22" s="95"/>
       <c r="X22" s="60"/>
       <c r="Y22" s="60"/>
       <c r="Z22" s="60"/>
@@ -3851,7 +3851,7 @@
       <c r="AN22" s="63"/>
     </row>
     <row r="23" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="165"/>
+      <c r="A23" s="163"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="22"/>
@@ -3863,17 +3863,17 @@
       <c r="J23" s="65"/>
       <c r="K23" s="65"/>
       <c r="L23" s="65"/>
-      <c r="M23" s="90"/>
-      <c r="N23" s="91"/>
+      <c r="M23" s="89"/>
+      <c r="N23" s="90"/>
       <c r="O23" s="65"/>
       <c r="P23" s="65"/>
       <c r="Q23" s="65"/>
       <c r="R23" s="65"/>
-      <c r="S23" s="90"/>
-      <c r="T23" s="91"/>
-      <c r="U23" s="90"/>
-      <c r="V23" s="95"/>
-      <c r="W23" s="91"/>
+      <c r="S23" s="89"/>
+      <c r="T23" s="90"/>
+      <c r="U23" s="89"/>
+      <c r="V23" s="98"/>
+      <c r="W23" s="90"/>
       <c r="X23" s="65"/>
       <c r="Y23" s="65"/>
       <c r="Z23" s="65"/>
@@ -3893,7 +3893,7 @@
       <c r="AN23" s="68"/>
     </row>
     <row r="24" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="165"/>
+      <c r="A24" s="163"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
@@ -3905,17 +3905,17 @@
       <c r="J24" s="60"/>
       <c r="K24" s="60"/>
       <c r="L24" s="60"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="88"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="95"/>
       <c r="O24" s="60"/>
       <c r="P24" s="60"/>
       <c r="Q24" s="60"/>
       <c r="R24" s="60"/>
-      <c r="S24" s="87"/>
-      <c r="T24" s="88"/>
-      <c r="U24" s="87"/>
-      <c r="V24" s="89"/>
-      <c r="W24" s="88"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="95"/>
+      <c r="U24" s="96"/>
+      <c r="V24" s="97"/>
+      <c r="W24" s="95"/>
       <c r="X24" s="60"/>
       <c r="Y24" s="60"/>
       <c r="Z24" s="60"/>
@@ -3935,7 +3935,7 @@
       <c r="AN24" s="63"/>
     </row>
     <row r="25" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="165"/>
+      <c r="A25" s="163"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="22"/>
@@ -3947,17 +3947,17 @@
       <c r="J25" s="65"/>
       <c r="K25" s="65"/>
       <c r="L25" s="65"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="91"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="90"/>
       <c r="O25" s="65"/>
       <c r="P25" s="65"/>
       <c r="Q25" s="65"/>
       <c r="R25" s="65"/>
-      <c r="S25" s="90"/>
-      <c r="T25" s="91"/>
-      <c r="U25" s="90"/>
-      <c r="V25" s="95"/>
-      <c r="W25" s="91"/>
+      <c r="S25" s="89"/>
+      <c r="T25" s="90"/>
+      <c r="U25" s="89"/>
+      <c r="V25" s="98"/>
+      <c r="W25" s="90"/>
       <c r="X25" s="65"/>
       <c r="Y25" s="65"/>
       <c r="Z25" s="65"/>
@@ -3977,7 +3977,7 @@
       <c r="AN25" s="68"/>
     </row>
     <row r="26" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="165"/>
+      <c r="A26" s="163"/>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
@@ -3989,17 +3989,17 @@
       <c r="J26" s="60"/>
       <c r="K26" s="60"/>
       <c r="L26" s="60"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="88"/>
+      <c r="M26" s="96"/>
+      <c r="N26" s="95"/>
       <c r="O26" s="60"/>
       <c r="P26" s="60"/>
       <c r="Q26" s="60"/>
       <c r="R26" s="60"/>
-      <c r="S26" s="87"/>
-      <c r="T26" s="88"/>
-      <c r="U26" s="87"/>
-      <c r="V26" s="89"/>
-      <c r="W26" s="88"/>
+      <c r="S26" s="96"/>
+      <c r="T26" s="95"/>
+      <c r="U26" s="96"/>
+      <c r="V26" s="97"/>
+      <c r="W26" s="95"/>
       <c r="X26" s="60"/>
       <c r="Y26" s="60"/>
       <c r="Z26" s="60"/>
@@ -4019,7 +4019,7 @@
       <c r="AN26" s="63"/>
     </row>
     <row r="27" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="165"/>
+      <c r="A27" s="163"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
       <c r="D27" s="22"/>
@@ -4031,17 +4031,17 @@
       <c r="J27" s="65"/>
       <c r="K27" s="65"/>
       <c r="L27" s="65"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="91"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="90"/>
       <c r="O27" s="65"/>
       <c r="P27" s="65"/>
       <c r="Q27" s="65"/>
       <c r="R27" s="65"/>
-      <c r="S27" s="90"/>
-      <c r="T27" s="91"/>
-      <c r="U27" s="90"/>
-      <c r="V27" s="95"/>
-      <c r="W27" s="91"/>
+      <c r="S27" s="89"/>
+      <c r="T27" s="90"/>
+      <c r="U27" s="89"/>
+      <c r="V27" s="98"/>
+      <c r="W27" s="90"/>
       <c r="X27" s="65"/>
       <c r="Y27" s="65"/>
       <c r="Z27" s="65"/>
@@ -4061,7 +4061,7 @@
       <c r="AN27" s="68"/>
     </row>
     <row r="28" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="165"/>
+      <c r="A28" s="163"/>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
@@ -4073,17 +4073,17 @@
       <c r="J28" s="60"/>
       <c r="K28" s="60"/>
       <c r="L28" s="60"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="88"/>
+      <c r="M28" s="96"/>
+      <c r="N28" s="95"/>
       <c r="O28" s="60"/>
       <c r="P28" s="60"/>
       <c r="Q28" s="60"/>
       <c r="R28" s="60"/>
-      <c r="S28" s="87"/>
-      <c r="T28" s="88"/>
-      <c r="U28" s="87"/>
-      <c r="V28" s="89"/>
-      <c r="W28" s="88"/>
+      <c r="S28" s="96"/>
+      <c r="T28" s="95"/>
+      <c r="U28" s="96"/>
+      <c r="V28" s="97"/>
+      <c r="W28" s="95"/>
       <c r="X28" s="60"/>
       <c r="Y28" s="60"/>
       <c r="Z28" s="60"/>
@@ -4103,7 +4103,7 @@
       <c r="AN28" s="63"/>
     </row>
     <row r="29" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="165"/>
+      <c r="A29" s="163"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="22"/>
@@ -4115,17 +4115,17 @@
       <c r="J29" s="65"/>
       <c r="K29" s="65"/>
       <c r="L29" s="65"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="91"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="90"/>
       <c r="O29" s="65"/>
       <c r="P29" s="65"/>
       <c r="Q29" s="65"/>
       <c r="R29" s="65"/>
-      <c r="S29" s="90"/>
-      <c r="T29" s="91"/>
-      <c r="U29" s="90"/>
-      <c r="V29" s="95"/>
-      <c r="W29" s="91"/>
+      <c r="S29" s="89"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="89"/>
+      <c r="V29" s="98"/>
+      <c r="W29" s="90"/>
       <c r="X29" s="65"/>
       <c r="Y29" s="65"/>
       <c r="Z29" s="65"/>
@@ -4145,7 +4145,7 @@
       <c r="AN29" s="68"/>
     </row>
     <row r="30" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="165"/>
+      <c r="A30" s="163"/>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
@@ -4157,17 +4157,17 @@
       <c r="J30" s="60"/>
       <c r="K30" s="60"/>
       <c r="L30" s="60"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="88"/>
+      <c r="M30" s="96"/>
+      <c r="N30" s="95"/>
       <c r="O30" s="60"/>
       <c r="P30" s="60"/>
       <c r="Q30" s="60"/>
       <c r="R30" s="60"/>
-      <c r="S30" s="87"/>
-      <c r="T30" s="88"/>
-      <c r="U30" s="87"/>
-      <c r="V30" s="89"/>
-      <c r="W30" s="88"/>
+      <c r="S30" s="96"/>
+      <c r="T30" s="95"/>
+      <c r="U30" s="96"/>
+      <c r="V30" s="97"/>
+      <c r="W30" s="95"/>
       <c r="X30" s="60"/>
       <c r="Y30" s="60"/>
       <c r="Z30" s="60"/>
@@ -4187,7 +4187,7 @@
       <c r="AN30" s="63"/>
     </row>
     <row r="31" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="165"/>
+      <c r="A31" s="163"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="22"/>
@@ -4199,17 +4199,17 @@
       <c r="J31" s="65"/>
       <c r="K31" s="65"/>
       <c r="L31" s="65"/>
-      <c r="M31" s="90"/>
-      <c r="N31" s="91"/>
+      <c r="M31" s="89"/>
+      <c r="N31" s="90"/>
       <c r="O31" s="65"/>
       <c r="P31" s="65"/>
       <c r="Q31" s="65"/>
       <c r="R31" s="65"/>
-      <c r="S31" s="90"/>
-      <c r="T31" s="91"/>
-      <c r="U31" s="90"/>
-      <c r="V31" s="95"/>
-      <c r="W31" s="91"/>
+      <c r="S31" s="89"/>
+      <c r="T31" s="90"/>
+      <c r="U31" s="89"/>
+      <c r="V31" s="98"/>
+      <c r="W31" s="90"/>
       <c r="X31" s="65"/>
       <c r="Y31" s="65"/>
       <c r="Z31" s="65"/>
@@ -4229,7 +4229,7 @@
       <c r="AN31" s="68"/>
     </row>
     <row r="32" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="165"/>
+      <c r="A32" s="163"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
@@ -4241,17 +4241,17 @@
       <c r="J32" s="60"/>
       <c r="K32" s="60"/>
       <c r="L32" s="60"/>
-      <c r="M32" s="87"/>
-      <c r="N32" s="88"/>
+      <c r="M32" s="96"/>
+      <c r="N32" s="95"/>
       <c r="O32" s="60"/>
       <c r="P32" s="60"/>
       <c r="Q32" s="60"/>
       <c r="R32" s="60"/>
-      <c r="S32" s="87"/>
-      <c r="T32" s="88"/>
-      <c r="U32" s="87"/>
-      <c r="V32" s="89"/>
-      <c r="W32" s="88"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="95"/>
+      <c r="U32" s="96"/>
+      <c r="V32" s="97"/>
+      <c r="W32" s="95"/>
       <c r="X32" s="60"/>
       <c r="Y32" s="60"/>
       <c r="Z32" s="60"/>
@@ -4271,7 +4271,7 @@
       <c r="AN32" s="63"/>
     </row>
     <row r="33" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="165"/>
+      <c r="A33" s="163"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="22"/>
@@ -4283,17 +4283,17 @@
       <c r="J33" s="65"/>
       <c r="K33" s="65"/>
       <c r="L33" s="65"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="91"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="90"/>
       <c r="O33" s="65"/>
       <c r="P33" s="65"/>
       <c r="Q33" s="65"/>
       <c r="R33" s="65"/>
-      <c r="S33" s="90"/>
-      <c r="T33" s="91"/>
-      <c r="U33" s="90"/>
-      <c r="V33" s="95"/>
-      <c r="W33" s="91"/>
+      <c r="S33" s="89"/>
+      <c r="T33" s="90"/>
+      <c r="U33" s="89"/>
+      <c r="V33" s="98"/>
+      <c r="W33" s="90"/>
       <c r="X33" s="65"/>
       <c r="Y33" s="65"/>
       <c r="Z33" s="65"/>
@@ -4313,7 +4313,7 @@
       <c r="AN33" s="68"/>
     </row>
     <row r="34" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="165"/>
+      <c r="A34" s="163"/>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="20"/>
@@ -4325,17 +4325,17 @@
       <c r="J34" s="60"/>
       <c r="K34" s="60"/>
       <c r="L34" s="60"/>
-      <c r="M34" s="87"/>
-      <c r="N34" s="88"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="95"/>
       <c r="O34" s="60"/>
       <c r="P34" s="60"/>
       <c r="Q34" s="60"/>
       <c r="R34" s="60"/>
-      <c r="S34" s="87"/>
-      <c r="T34" s="88"/>
-      <c r="U34" s="87"/>
-      <c r="V34" s="89"/>
-      <c r="W34" s="88"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="95"/>
+      <c r="U34" s="96"/>
+      <c r="V34" s="97"/>
+      <c r="W34" s="95"/>
       <c r="X34" s="60"/>
       <c r="Y34" s="60"/>
       <c r="Z34" s="60"/>
@@ -4355,7 +4355,7 @@
       <c r="AN34" s="63"/>
     </row>
     <row r="35" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="165"/>
+      <c r="A35" s="163"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
       <c r="D35" s="22"/>
@@ -4367,17 +4367,17 @@
       <c r="J35" s="65"/>
       <c r="K35" s="65"/>
       <c r="L35" s="65"/>
-      <c r="M35" s="90"/>
-      <c r="N35" s="91"/>
+      <c r="M35" s="89"/>
+      <c r="N35" s="90"/>
       <c r="O35" s="65"/>
       <c r="P35" s="65"/>
       <c r="Q35" s="65"/>
       <c r="R35" s="65"/>
-      <c r="S35" s="90"/>
-      <c r="T35" s="91"/>
-      <c r="U35" s="90"/>
-      <c r="V35" s="95"/>
-      <c r="W35" s="91"/>
+      <c r="S35" s="89"/>
+      <c r="T35" s="90"/>
+      <c r="U35" s="89"/>
+      <c r="V35" s="98"/>
+      <c r="W35" s="90"/>
       <c r="X35" s="65"/>
       <c r="Y35" s="65"/>
       <c r="Z35" s="65"/>
@@ -4397,7 +4397,7 @@
       <c r="AN35" s="68"/>
     </row>
     <row r="36" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="165"/>
+      <c r="A36" s="163"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="20"/>
@@ -4409,17 +4409,17 @@
       <c r="J36" s="60"/>
       <c r="K36" s="60"/>
       <c r="L36" s="60"/>
-      <c r="M36" s="87"/>
-      <c r="N36" s="88"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="95"/>
       <c r="O36" s="60"/>
       <c r="P36" s="60"/>
       <c r="Q36" s="60"/>
       <c r="R36" s="60"/>
-      <c r="S36" s="87"/>
-      <c r="T36" s="88"/>
-      <c r="U36" s="87"/>
-      <c r="V36" s="89"/>
-      <c r="W36" s="88"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="95"/>
+      <c r="U36" s="96"/>
+      <c r="V36" s="97"/>
+      <c r="W36" s="95"/>
       <c r="X36" s="60"/>
       <c r="Y36" s="60"/>
       <c r="Z36" s="60"/>
@@ -4439,7 +4439,7 @@
       <c r="AN36" s="63"/>
     </row>
     <row r="37" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="165"/>
+      <c r="A37" s="163"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
       <c r="D37" s="22"/>
@@ -4451,17 +4451,17 @@
       <c r="J37" s="65"/>
       <c r="K37" s="65"/>
       <c r="L37" s="65"/>
-      <c r="M37" s="90"/>
-      <c r="N37" s="91"/>
+      <c r="M37" s="89"/>
+      <c r="N37" s="90"/>
       <c r="O37" s="65"/>
       <c r="P37" s="65"/>
       <c r="Q37" s="65"/>
       <c r="R37" s="65"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="91"/>
-      <c r="U37" s="90"/>
-      <c r="V37" s="95"/>
-      <c r="W37" s="91"/>
+      <c r="S37" s="89"/>
+      <c r="T37" s="90"/>
+      <c r="U37" s="89"/>
+      <c r="V37" s="98"/>
+      <c r="W37" s="90"/>
       <c r="X37" s="65"/>
       <c r="Y37" s="65"/>
       <c r="Z37" s="65"/>
@@ -4481,7 +4481,7 @@
       <c r="AN37" s="68"/>
     </row>
     <row r="38" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="165"/>
+      <c r="A38" s="163"/>
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
       <c r="D38" s="20"/>
@@ -4493,17 +4493,17 @@
       <c r="J38" s="60"/>
       <c r="K38" s="60"/>
       <c r="L38" s="60"/>
-      <c r="M38" s="87"/>
-      <c r="N38" s="88"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="95"/>
       <c r="O38" s="60"/>
       <c r="P38" s="60"/>
       <c r="Q38" s="60"/>
       <c r="R38" s="60"/>
-      <c r="S38" s="87"/>
-      <c r="T38" s="88"/>
-      <c r="U38" s="87"/>
-      <c r="V38" s="89"/>
-      <c r="W38" s="88"/>
+      <c r="S38" s="96"/>
+      <c r="T38" s="95"/>
+      <c r="U38" s="96"/>
+      <c r="V38" s="97"/>
+      <c r="W38" s="95"/>
       <c r="X38" s="60"/>
       <c r="Y38" s="60"/>
       <c r="Z38" s="60"/>
@@ -4523,7 +4523,7 @@
       <c r="AN38" s="63"/>
     </row>
     <row r="39" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="165"/>
+      <c r="A39" s="163"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
       <c r="D39" s="22"/>
@@ -4535,17 +4535,17 @@
       <c r="J39" s="65"/>
       <c r="K39" s="65"/>
       <c r="L39" s="65"/>
-      <c r="M39" s="90"/>
-      <c r="N39" s="91"/>
+      <c r="M39" s="89"/>
+      <c r="N39" s="90"/>
       <c r="O39" s="65"/>
       <c r="P39" s="65"/>
       <c r="Q39" s="65"/>
       <c r="R39" s="65"/>
-      <c r="S39" s="90"/>
-      <c r="T39" s="91"/>
-      <c r="U39" s="90"/>
-      <c r="V39" s="95"/>
-      <c r="W39" s="91"/>
+      <c r="S39" s="89"/>
+      <c r="T39" s="90"/>
+      <c r="U39" s="89"/>
+      <c r="V39" s="98"/>
+      <c r="W39" s="90"/>
       <c r="X39" s="65"/>
       <c r="Y39" s="65"/>
       <c r="Z39" s="65"/>
@@ -4565,7 +4565,7 @@
       <c r="AN39" s="68"/>
     </row>
     <row r="40" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="165"/>
+      <c r="A40" s="163"/>
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
@@ -4577,17 +4577,17 @@
       <c r="J40" s="60"/>
       <c r="K40" s="60"/>
       <c r="L40" s="60"/>
-      <c r="M40" s="87"/>
-      <c r="N40" s="88"/>
+      <c r="M40" s="96"/>
+      <c r="N40" s="95"/>
       <c r="O40" s="60"/>
       <c r="P40" s="60"/>
       <c r="Q40" s="60"/>
       <c r="R40" s="60"/>
-      <c r="S40" s="87"/>
-      <c r="T40" s="88"/>
-      <c r="U40" s="87"/>
-      <c r="V40" s="89"/>
-      <c r="W40" s="88"/>
+      <c r="S40" s="96"/>
+      <c r="T40" s="95"/>
+      <c r="U40" s="96"/>
+      <c r="V40" s="97"/>
+      <c r="W40" s="95"/>
       <c r="X40" s="60"/>
       <c r="Y40" s="60"/>
       <c r="Z40" s="60"/>
@@ -4607,7 +4607,7 @@
       <c r="AN40" s="63"/>
     </row>
     <row r="41" spans="1:40" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="166"/>
+      <c r="A41" s="164"/>
       <c r="B41" s="51"/>
       <c r="C41" s="51"/>
       <c r="D41" s="52"/>
@@ -4619,17 +4619,17 @@
       <c r="J41" s="70"/>
       <c r="K41" s="70"/>
       <c r="L41" s="70"/>
-      <c r="M41" s="194"/>
-      <c r="N41" s="195"/>
+      <c r="M41" s="99"/>
+      <c r="N41" s="100"/>
       <c r="O41" s="70"/>
       <c r="P41" s="70"/>
       <c r="Q41" s="70"/>
       <c r="R41" s="70"/>
-      <c r="S41" s="194"/>
-      <c r="T41" s="195"/>
-      <c r="U41" s="194"/>
-      <c r="V41" s="230"/>
-      <c r="W41" s="195"/>
+      <c r="S41" s="99"/>
+      <c r="T41" s="100"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="138"/>
+      <c r="W41" s="100"/>
       <c r="X41" s="70"/>
       <c r="Y41" s="70"/>
       <c r="Z41" s="70"/>
@@ -4661,17 +4661,17 @@
       <c r="J42" s="74"/>
       <c r="K42" s="74"/>
       <c r="L42" s="74"/>
-      <c r="M42" s="229"/>
-      <c r="N42" s="229"/>
+      <c r="M42" s="137"/>
+      <c r="N42" s="137"/>
       <c r="O42" s="74"/>
       <c r="P42" s="74"/>
       <c r="Q42" s="74"/>
       <c r="R42" s="74"/>
       <c r="S42" s="74"/>
       <c r="T42" s="74"/>
-      <c r="U42" s="229"/>
-      <c r="V42" s="229"/>
-      <c r="W42" s="229"/>
+      <c r="U42" s="137"/>
+      <c r="V42" s="137"/>
+      <c r="W42" s="137"/>
       <c r="X42" s="74"/>
       <c r="Y42" s="74"/>
       <c r="Z42" s="74"/>
@@ -4691,13 +4691,13 @@
       <c r="AN42" s="74"/>
     </row>
     <row r="43" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="177" t="s">
+      <c r="A43" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="108"/>
-      <c r="C43" s="108"/>
-      <c r="D43" s="108"/>
-      <c r="E43" s="178"/>
+      <c r="B43" s="144"/>
+      <c r="C43" s="144"/>
+      <c r="D43" s="144"/>
+      <c r="E43" s="145"/>
       <c r="F43" s="29"/>
       <c r="G43" s="75"/>
       <c r="H43" s="76"/>
@@ -4705,17 +4705,17 @@
       <c r="J43" s="76"/>
       <c r="K43" s="76"/>
       <c r="L43" s="76"/>
-      <c r="M43" s="184"/>
-      <c r="N43" s="185"/>
+      <c r="M43" s="152"/>
+      <c r="N43" s="153"/>
       <c r="O43" s="76"/>
       <c r="P43" s="76"/>
       <c r="Q43" s="76"/>
       <c r="R43" s="76"/>
-      <c r="S43" s="185"/>
-      <c r="T43" s="185"/>
-      <c r="U43" s="184"/>
-      <c r="V43" s="185"/>
-      <c r="W43" s="185"/>
+      <c r="S43" s="153"/>
+      <c r="T43" s="153"/>
+      <c r="U43" s="152"/>
+      <c r="V43" s="153"/>
+      <c r="W43" s="153"/>
       <c r="X43" s="76"/>
       <c r="Y43" s="76"/>
       <c r="Z43" s="76"/>
@@ -4735,11 +4735,11 @@
       <c r="AN43" s="78"/>
     </row>
     <row r="44" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="179"/>
-      <c r="B44" s="111"/>
-      <c r="C44" s="111"/>
-      <c r="D44" s="111"/>
-      <c r="E44" s="180"/>
+      <c r="A44" s="146"/>
+      <c r="B44" s="147"/>
+      <c r="C44" s="147"/>
+      <c r="D44" s="147"/>
+      <c r="E44" s="148"/>
       <c r="F44" s="30"/>
       <c r="G44" s="79"/>
       <c r="H44" s="80"/>
@@ -4747,17 +4747,17 @@
       <c r="J44" s="80"/>
       <c r="K44" s="80"/>
       <c r="L44" s="80"/>
-      <c r="M44" s="91"/>
-      <c r="N44" s="186"/>
+      <c r="M44" s="90"/>
+      <c r="N44" s="93"/>
       <c r="O44" s="80"/>
       <c r="P44" s="80"/>
       <c r="Q44" s="80"/>
       <c r="R44" s="80"/>
-      <c r="S44" s="186"/>
-      <c r="T44" s="186"/>
-      <c r="U44" s="91"/>
-      <c r="V44" s="186"/>
-      <c r="W44" s="186"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
       <c r="X44" s="80"/>
       <c r="Y44" s="80"/>
       <c r="Z44" s="80"/>
@@ -4777,11 +4777,11 @@
       <c r="AN44" s="82"/>
     </row>
     <row r="45" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="179"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="111"/>
-      <c r="D45" s="111"/>
-      <c r="E45" s="180"/>
+      <c r="A45" s="146"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="147"/>
+      <c r="D45" s="147"/>
+      <c r="E45" s="148"/>
       <c r="F45" s="31"/>
       <c r="G45" s="59"/>
       <c r="H45" s="60"/>
@@ -4789,17 +4789,17 @@
       <c r="J45" s="60"/>
       <c r="K45" s="60"/>
       <c r="L45" s="60"/>
-      <c r="M45" s="88"/>
-      <c r="N45" s="187"/>
+      <c r="M45" s="95"/>
+      <c r="N45" s="94"/>
       <c r="O45" s="60"/>
       <c r="P45" s="60"/>
       <c r="Q45" s="60"/>
       <c r="R45" s="60"/>
-      <c r="S45" s="187"/>
-      <c r="T45" s="187"/>
-      <c r="U45" s="88"/>
-      <c r="V45" s="187"/>
-      <c r="W45" s="187"/>
+      <c r="S45" s="94"/>
+      <c r="T45" s="94"/>
+      <c r="U45" s="95"/>
+      <c r="V45" s="94"/>
+      <c r="W45" s="94"/>
       <c r="X45" s="60"/>
       <c r="Y45" s="60"/>
       <c r="Z45" s="60"/>
@@ -4819,11 +4819,11 @@
       <c r="AN45" s="63"/>
     </row>
     <row r="46" spans="1:40" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="179"/>
-      <c r="B46" s="111"/>
-      <c r="C46" s="111"/>
-      <c r="D46" s="111"/>
-      <c r="E46" s="180"/>
+      <c r="A46" s="146"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="147"/>
+      <c r="D46" s="147"/>
+      <c r="E46" s="148"/>
       <c r="F46" s="30"/>
       <c r="G46" s="79"/>
       <c r="H46" s="80"/>
@@ -4831,17 +4831,17 @@
       <c r="J46" s="80"/>
       <c r="K46" s="80"/>
       <c r="L46" s="80"/>
-      <c r="M46" s="91"/>
-      <c r="N46" s="186"/>
+      <c r="M46" s="90"/>
+      <c r="N46" s="93"/>
       <c r="O46" s="80"/>
       <c r="P46" s="80"/>
       <c r="Q46" s="80"/>
       <c r="R46" s="80"/>
-      <c r="S46" s="186"/>
-      <c r="T46" s="186"/>
-      <c r="U46" s="91"/>
-      <c r="V46" s="186"/>
-      <c r="W46" s="186"/>
+      <c r="S46" s="93"/>
+      <c r="T46" s="93"/>
+      <c r="U46" s="90"/>
+      <c r="V46" s="93"/>
+      <c r="W46" s="93"/>
       <c r="X46" s="80"/>
       <c r="Y46" s="80"/>
       <c r="Z46" s="80"/>
@@ -4861,11 +4861,11 @@
       <c r="AN46" s="82"/>
     </row>
     <row r="47" spans="1:40" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="181"/>
-      <c r="B47" s="182"/>
-      <c r="C47" s="182"/>
-      <c r="D47" s="182"/>
-      <c r="E47" s="183"/>
+      <c r="A47" s="149"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="150"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="151"/>
       <c r="F47" s="32"/>
       <c r="G47" s="83"/>
       <c r="H47" s="84"/>
@@ -4873,17 +4873,17 @@
       <c r="J47" s="84"/>
       <c r="K47" s="84"/>
       <c r="L47" s="84"/>
-      <c r="M47" s="227"/>
-      <c r="N47" s="228"/>
+      <c r="M47" s="135"/>
+      <c r="N47" s="136"/>
       <c r="O47" s="84"/>
       <c r="P47" s="84"/>
       <c r="Q47" s="84"/>
       <c r="R47" s="84"/>
-      <c r="S47" s="228"/>
-      <c r="T47" s="228"/>
-      <c r="U47" s="227"/>
-      <c r="V47" s="228"/>
-      <c r="W47" s="228"/>
+      <c r="S47" s="136"/>
+      <c r="T47" s="136"/>
+      <c r="U47" s="135"/>
+      <c r="V47" s="136"/>
+      <c r="W47" s="136"/>
       <c r="X47" s="84"/>
       <c r="Y47" s="84"/>
       <c r="Z47" s="84"/>
@@ -4927,10 +4927,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M48" s="176">
+      <c r="M48" s="142">
+        <f>SUM(M13:N47)</f>
         <v>0</v>
       </c>
-      <c r="N48" s="176"/>
+      <c r="N48" s="142"/>
       <c r="O48" s="53">
         <f>SUM(O13:O47)</f>
         <v>0</v>
@@ -4947,17 +4948,17 @@
         <f>SUM(R13:R47)</f>
         <v>0</v>
       </c>
-      <c r="S48" s="176">
+      <c r="S48" s="142">
         <f>SUM(S13:T47)</f>
         <v>0</v>
       </c>
-      <c r="T48" s="176"/>
-      <c r="U48" s="176">
+      <c r="T48" s="142"/>
+      <c r="U48" s="142">
         <f>SUM(U13:W47)</f>
         <v>0</v>
       </c>
-      <c r="V48" s="176"/>
-      <c r="W48" s="176"/>
+      <c r="V48" s="142"/>
+      <c r="W48" s="142"/>
       <c r="X48" s="53">
         <f t="shared" ref="X48:AN48" si="1">SUM(X13:X47)</f>
         <v>0</v>
@@ -5028,104 +5029,104 @@
       </c>
     </row>
     <row r="49" spans="1:60" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="170" t="s">
+      <c r="A49" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="188">
+      <c r="B49" s="154">
         <v>13</v>
       </c>
-      <c r="C49" s="189"/>
-      <c r="D49" s="173" t="s">
+      <c r="C49" s="155"/>
+      <c r="D49" s="139" t="s">
         <v>16</v>
       </c>
-      <c r="E49" s="174"/>
-      <c r="F49" s="174"/>
-      <c r="G49" s="174"/>
-      <c r="H49" s="174"/>
-      <c r="I49" s="174"/>
-      <c r="J49" s="174"/>
-      <c r="K49" s="174"/>
-      <c r="L49" s="174"/>
-      <c r="M49" s="174"/>
-      <c r="N49" s="174"/>
-      <c r="O49" s="174"/>
-      <c r="P49" s="174"/>
-      <c r="Q49" s="174"/>
-      <c r="R49" s="174"/>
-      <c r="S49" s="174"/>
-      <c r="T49" s="174"/>
-      <c r="U49" s="174"/>
-      <c r="V49" s="174"/>
-      <c r="W49" s="174"/>
-      <c r="X49" s="174"/>
-      <c r="Y49" s="174"/>
-      <c r="Z49" s="174"/>
-      <c r="AA49" s="174"/>
-      <c r="AB49" s="174"/>
-      <c r="AC49" s="174"/>
-      <c r="AD49" s="175"/>
-      <c r="AE49" s="170" t="s">
+      <c r="E49" s="140"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="140"/>
+      <c r="I49" s="140"/>
+      <c r="J49" s="140"/>
+      <c r="K49" s="140"/>
+      <c r="L49" s="140"/>
+      <c r="M49" s="140"/>
+      <c r="N49" s="140"/>
+      <c r="O49" s="140"/>
+      <c r="P49" s="140"/>
+      <c r="Q49" s="140"/>
+      <c r="R49" s="140"/>
+      <c r="S49" s="140"/>
+      <c r="T49" s="140"/>
+      <c r="U49" s="140"/>
+      <c r="V49" s="140"/>
+      <c r="W49" s="140"/>
+      <c r="X49" s="140"/>
+      <c r="Y49" s="140"/>
+      <c r="Z49" s="140"/>
+      <c r="AA49" s="140"/>
+      <c r="AB49" s="140"/>
+      <c r="AC49" s="140"/>
+      <c r="AD49" s="141"/>
+      <c r="AE49" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="AF49" s="214">
+      <c r="AF49" s="122">
         <v>34</v>
       </c>
-      <c r="AG49" s="215" t="s">
+      <c r="AG49" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="AH49" s="216"/>
-      <c r="AI49" s="216"/>
-      <c r="AJ49" s="216"/>
-      <c r="AK49" s="216"/>
-      <c r="AL49" s="216"/>
-      <c r="AM49" s="216"/>
-      <c r="AN49" s="217"/>
+      <c r="AH49" s="124"/>
+      <c r="AI49" s="124"/>
+      <c r="AJ49" s="124"/>
+      <c r="AK49" s="124"/>
+      <c r="AL49" s="124"/>
+      <c r="AM49" s="124"/>
+      <c r="AN49" s="125"/>
     </row>
     <row r="50" spans="1:60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="171"/>
-      <c r="B50" s="190">
+      <c r="A50" s="120"/>
+      <c r="B50" s="156">
         <v>16</v>
       </c>
-      <c r="C50" s="191"/>
-      <c r="D50" s="221" t="s">
+      <c r="C50" s="157"/>
+      <c r="D50" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="E50" s="222"/>
-      <c r="F50" s="222"/>
-      <c r="G50" s="222"/>
-      <c r="H50" s="222"/>
-      <c r="I50" s="222"/>
-      <c r="J50" s="222"/>
-      <c r="K50" s="222"/>
-      <c r="L50" s="222"/>
-      <c r="M50" s="222"/>
-      <c r="N50" s="222"/>
-      <c r="O50" s="222"/>
-      <c r="P50" s="222"/>
-      <c r="Q50" s="222"/>
-      <c r="R50" s="222"/>
-      <c r="S50" s="222"/>
-      <c r="T50" s="222"/>
-      <c r="U50" s="222"/>
-      <c r="V50" s="222"/>
-      <c r="W50" s="222"/>
-      <c r="X50" s="222"/>
-      <c r="Y50" s="222"/>
-      <c r="Z50" s="222"/>
-      <c r="AA50" s="222"/>
-      <c r="AB50" s="222"/>
-      <c r="AC50" s="222"/>
-      <c r="AD50" s="223"/>
-      <c r="AE50" s="171"/>
-      <c r="AF50" s="201"/>
-      <c r="AG50" s="218"/>
-      <c r="AH50" s="219"/>
-      <c r="AI50" s="219"/>
-      <c r="AJ50" s="219"/>
-      <c r="AK50" s="219"/>
-      <c r="AL50" s="219"/>
-      <c r="AM50" s="219"/>
-      <c r="AN50" s="220"/>
+      <c r="E50" s="130"/>
+      <c r="F50" s="130"/>
+      <c r="G50" s="130"/>
+      <c r="H50" s="130"/>
+      <c r="I50" s="130"/>
+      <c r="J50" s="130"/>
+      <c r="K50" s="130"/>
+      <c r="L50" s="130"/>
+      <c r="M50" s="130"/>
+      <c r="N50" s="130"/>
+      <c r="O50" s="130"/>
+      <c r="P50" s="130"/>
+      <c r="Q50" s="130"/>
+      <c r="R50" s="130"/>
+      <c r="S50" s="130"/>
+      <c r="T50" s="130"/>
+      <c r="U50" s="130"/>
+      <c r="V50" s="130"/>
+      <c r="W50" s="130"/>
+      <c r="X50" s="130"/>
+      <c r="Y50" s="130"/>
+      <c r="Z50" s="130"/>
+      <c r="AA50" s="130"/>
+      <c r="AB50" s="130"/>
+      <c r="AC50" s="130"/>
+      <c r="AD50" s="131"/>
+      <c r="AE50" s="120"/>
+      <c r="AF50" s="106"/>
+      <c r="AG50" s="126"/>
+      <c r="AH50" s="127"/>
+      <c r="AI50" s="127"/>
+      <c r="AJ50" s="127"/>
+      <c r="AK50" s="127"/>
+      <c r="AL50" s="127"/>
+      <c r="AM50" s="127"/>
+      <c r="AN50" s="128"/>
       <c r="AO50" s="38"/>
       <c r="AP50" s="38"/>
       <c r="AQ50" s="38"/>
@@ -5148,54 +5149,54 @@
       <c r="BH50" s="16"/>
     </row>
     <row r="51" spans="1:60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="171"/>
-      <c r="B51" s="190">
+      <c r="A51" s="120"/>
+      <c r="B51" s="156">
         <v>19</v>
       </c>
-      <c r="C51" s="191"/>
-      <c r="D51" s="221" t="s">
+      <c r="C51" s="157"/>
+      <c r="D51" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="222"/>
-      <c r="F51" s="222"/>
-      <c r="G51" s="222"/>
-      <c r="H51" s="222"/>
-      <c r="I51" s="222"/>
-      <c r="J51" s="222"/>
-      <c r="K51" s="222"/>
-      <c r="L51" s="222"/>
-      <c r="M51" s="222"/>
-      <c r="N51" s="222"/>
-      <c r="O51" s="222"/>
-      <c r="P51" s="222"/>
-      <c r="Q51" s="222"/>
-      <c r="R51" s="222"/>
-      <c r="S51" s="222"/>
-      <c r="T51" s="222"/>
-      <c r="U51" s="222"/>
-      <c r="V51" s="222"/>
-      <c r="W51" s="222"/>
-      <c r="X51" s="222"/>
-      <c r="Y51" s="222"/>
-      <c r="Z51" s="222"/>
-      <c r="AA51" s="222"/>
-      <c r="AB51" s="222"/>
-      <c r="AC51" s="222"/>
-      <c r="AD51" s="223"/>
-      <c r="AE51" s="171"/>
-      <c r="AF51" s="201">
+      <c r="E51" s="130"/>
+      <c r="F51" s="130"/>
+      <c r="G51" s="130"/>
+      <c r="H51" s="130"/>
+      <c r="I51" s="130"/>
+      <c r="J51" s="130"/>
+      <c r="K51" s="130"/>
+      <c r="L51" s="130"/>
+      <c r="M51" s="130"/>
+      <c r="N51" s="130"/>
+      <c r="O51" s="130"/>
+      <c r="P51" s="130"/>
+      <c r="Q51" s="130"/>
+      <c r="R51" s="130"/>
+      <c r="S51" s="130"/>
+      <c r="T51" s="130"/>
+      <c r="U51" s="130"/>
+      <c r="V51" s="130"/>
+      <c r="W51" s="130"/>
+      <c r="X51" s="130"/>
+      <c r="Y51" s="130"/>
+      <c r="Z51" s="130"/>
+      <c r="AA51" s="130"/>
+      <c r="AB51" s="130"/>
+      <c r="AC51" s="130"/>
+      <c r="AD51" s="131"/>
+      <c r="AE51" s="120"/>
+      <c r="AF51" s="106">
         <v>35</v>
       </c>
-      <c r="AG51" s="203" t="s">
+      <c r="AG51" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="AH51" s="204"/>
-      <c r="AI51" s="204"/>
-      <c r="AJ51" s="204"/>
-      <c r="AK51" s="204"/>
-      <c r="AL51" s="204"/>
-      <c r="AM51" s="204"/>
-      <c r="AN51" s="205"/>
+      <c r="AH51" s="109"/>
+      <c r="AI51" s="109"/>
+      <c r="AJ51" s="109"/>
+      <c r="AK51" s="109"/>
+      <c r="AL51" s="109"/>
+      <c r="AM51" s="109"/>
+      <c r="AN51" s="110"/>
       <c r="AO51" s="38"/>
       <c r="AP51" s="38"/>
       <c r="AQ51" s="38"/>
@@ -5218,50 +5219,50 @@
       <c r="BH51" s="16"/>
     </row>
     <row r="52" spans="1:60" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="171"/>
-      <c r="B52" s="190">
+      <c r="A52" s="120"/>
+      <c r="B52" s="156">
         <v>23</v>
       </c>
-      <c r="C52" s="191"/>
-      <c r="D52" s="221" t="s">
+      <c r="C52" s="157"/>
+      <c r="D52" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="222"/>
-      <c r="F52" s="222"/>
-      <c r="G52" s="222"/>
-      <c r="H52" s="222"/>
-      <c r="I52" s="222"/>
-      <c r="J52" s="222"/>
-      <c r="K52" s="222"/>
-      <c r="L52" s="222"/>
-      <c r="M52" s="222"/>
-      <c r="N52" s="222"/>
-      <c r="O52" s="222"/>
-      <c r="P52" s="222"/>
-      <c r="Q52" s="222"/>
-      <c r="R52" s="222"/>
-      <c r="S52" s="222"/>
-      <c r="T52" s="222"/>
-      <c r="U52" s="222"/>
-      <c r="V52" s="222"/>
-      <c r="W52" s="222"/>
-      <c r="X52" s="222"/>
-      <c r="Y52" s="222"/>
-      <c r="Z52" s="222"/>
-      <c r="AA52" s="222"/>
-      <c r="AB52" s="222"/>
-      <c r="AC52" s="222"/>
-      <c r="AD52" s="223"/>
-      <c r="AE52" s="171"/>
-      <c r="AF52" s="201"/>
-      <c r="AG52" s="218"/>
-      <c r="AH52" s="219"/>
-      <c r="AI52" s="219"/>
-      <c r="AJ52" s="219"/>
-      <c r="AK52" s="219"/>
-      <c r="AL52" s="219"/>
-      <c r="AM52" s="219"/>
-      <c r="AN52" s="220"/>
+      <c r="E52" s="130"/>
+      <c r="F52" s="130"/>
+      <c r="G52" s="130"/>
+      <c r="H52" s="130"/>
+      <c r="I52" s="130"/>
+      <c r="J52" s="130"/>
+      <c r="K52" s="130"/>
+      <c r="L52" s="130"/>
+      <c r="M52" s="130"/>
+      <c r="N52" s="130"/>
+      <c r="O52" s="130"/>
+      <c r="P52" s="130"/>
+      <c r="Q52" s="130"/>
+      <c r="R52" s="130"/>
+      <c r="S52" s="130"/>
+      <c r="T52" s="130"/>
+      <c r="U52" s="130"/>
+      <c r="V52" s="130"/>
+      <c r="W52" s="130"/>
+      <c r="X52" s="130"/>
+      <c r="Y52" s="130"/>
+      <c r="Z52" s="130"/>
+      <c r="AA52" s="130"/>
+      <c r="AB52" s="130"/>
+      <c r="AC52" s="130"/>
+      <c r="AD52" s="131"/>
+      <c r="AE52" s="120"/>
+      <c r="AF52" s="106"/>
+      <c r="AG52" s="126"/>
+      <c r="AH52" s="127"/>
+      <c r="AI52" s="127"/>
+      <c r="AJ52" s="127"/>
+      <c r="AK52" s="127"/>
+      <c r="AL52" s="127"/>
+      <c r="AM52" s="127"/>
+      <c r="AN52" s="128"/>
       <c r="AO52" s="38"/>
       <c r="AP52" s="38"/>
       <c r="AQ52" s="38"/>
@@ -5284,54 +5285,54 @@
       <c r="BH52" s="16"/>
     </row>
     <row r="53" spans="1:60" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="171"/>
-      <c r="B53" s="190">
+      <c r="A53" s="120"/>
+      <c r="B53" s="156">
         <v>24</v>
       </c>
-      <c r="C53" s="191"/>
-      <c r="D53" s="221" t="s">
+      <c r="C53" s="157"/>
+      <c r="D53" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="222"/>
-      <c r="F53" s="222"/>
-      <c r="G53" s="222"/>
-      <c r="H53" s="222"/>
-      <c r="I53" s="222"/>
-      <c r="J53" s="222"/>
-      <c r="K53" s="222"/>
-      <c r="L53" s="222"/>
-      <c r="M53" s="222"/>
-      <c r="N53" s="222"/>
-      <c r="O53" s="222"/>
-      <c r="P53" s="222"/>
-      <c r="Q53" s="222"/>
-      <c r="R53" s="222"/>
-      <c r="S53" s="222"/>
-      <c r="T53" s="222"/>
-      <c r="U53" s="222"/>
-      <c r="V53" s="222"/>
-      <c r="W53" s="222"/>
-      <c r="X53" s="222"/>
-      <c r="Y53" s="222"/>
-      <c r="Z53" s="222"/>
-      <c r="AA53" s="222"/>
-      <c r="AB53" s="222"/>
-      <c r="AC53" s="222"/>
-      <c r="AD53" s="223"/>
-      <c r="AE53" s="171"/>
-      <c r="AF53" s="201">
+      <c r="E53" s="130"/>
+      <c r="F53" s="130"/>
+      <c r="G53" s="130"/>
+      <c r="H53" s="130"/>
+      <c r="I53" s="130"/>
+      <c r="J53" s="130"/>
+      <c r="K53" s="130"/>
+      <c r="L53" s="130"/>
+      <c r="M53" s="130"/>
+      <c r="N53" s="130"/>
+      <c r="O53" s="130"/>
+      <c r="P53" s="130"/>
+      <c r="Q53" s="130"/>
+      <c r="R53" s="130"/>
+      <c r="S53" s="130"/>
+      <c r="T53" s="130"/>
+      <c r="U53" s="130"/>
+      <c r="V53" s="130"/>
+      <c r="W53" s="130"/>
+      <c r="X53" s="130"/>
+      <c r="Y53" s="130"/>
+      <c r="Z53" s="130"/>
+      <c r="AA53" s="130"/>
+      <c r="AB53" s="130"/>
+      <c r="AC53" s="130"/>
+      <c r="AD53" s="131"/>
+      <c r="AE53" s="120"/>
+      <c r="AF53" s="106">
         <v>36</v>
       </c>
-      <c r="AG53" s="224" t="s">
+      <c r="AG53" s="132" t="s">
         <v>5</v>
       </c>
-      <c r="AH53" s="225"/>
-      <c r="AI53" s="225"/>
-      <c r="AJ53" s="225"/>
-      <c r="AK53" s="225"/>
-      <c r="AL53" s="225"/>
-      <c r="AM53" s="225"/>
-      <c r="AN53" s="226"/>
+      <c r="AH53" s="133"/>
+      <c r="AI53" s="133"/>
+      <c r="AJ53" s="133"/>
+      <c r="AK53" s="133"/>
+      <c r="AL53" s="133"/>
+      <c r="AM53" s="133"/>
+      <c r="AN53" s="134"/>
       <c r="AO53" s="35"/>
       <c r="AP53" s="35"/>
       <c r="AQ53" s="35"/>
@@ -5354,150 +5355,326 @@
       <c r="BH53" s="16"/>
     </row>
     <row r="54" spans="1:60" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="171"/>
-      <c r="B54" s="190">
+      <c r="A54" s="120"/>
+      <c r="B54" s="156">
         <v>50</v>
       </c>
-      <c r="C54" s="191"/>
-      <c r="D54" s="196" t="s">
+      <c r="C54" s="157"/>
+      <c r="D54" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="E54" s="197"/>
-      <c r="F54" s="198"/>
-      <c r="G54" s="198"/>
-      <c r="H54" s="198"/>
-      <c r="I54" s="198"/>
-      <c r="J54" s="198"/>
-      <c r="K54" s="198"/>
-      <c r="L54" s="198"/>
-      <c r="M54" s="198"/>
-      <c r="N54" s="198"/>
-      <c r="O54" s="198"/>
-      <c r="P54" s="198"/>
-      <c r="Q54" s="198"/>
-      <c r="R54" s="198"/>
-      <c r="S54" s="198"/>
-      <c r="T54" s="198"/>
-      <c r="U54" s="198"/>
-      <c r="V54" s="198"/>
-      <c r="W54" s="198"/>
-      <c r="X54" s="198"/>
-      <c r="Y54" s="198"/>
-      <c r="Z54" s="198"/>
-      <c r="AA54" s="198"/>
-      <c r="AB54" s="198"/>
-      <c r="AC54" s="199"/>
-      <c r="AD54" s="200"/>
-      <c r="AE54" s="171"/>
-      <c r="AF54" s="201"/>
-      <c r="AG54" s="218"/>
-      <c r="AH54" s="219"/>
-      <c r="AI54" s="219"/>
-      <c r="AJ54" s="219"/>
-      <c r="AK54" s="219"/>
-      <c r="AL54" s="219"/>
-      <c r="AM54" s="219"/>
-      <c r="AN54" s="220"/>
+      <c r="E54" s="102"/>
+      <c r="F54" s="103"/>
+      <c r="G54" s="103"/>
+      <c r="H54" s="103"/>
+      <c r="I54" s="103"/>
+      <c r="J54" s="103"/>
+      <c r="K54" s="103"/>
+      <c r="L54" s="103"/>
+      <c r="M54" s="103"/>
+      <c r="N54" s="103"/>
+      <c r="O54" s="103"/>
+      <c r="P54" s="103"/>
+      <c r="Q54" s="103"/>
+      <c r="R54" s="103"/>
+      <c r="S54" s="103"/>
+      <c r="T54" s="103"/>
+      <c r="U54" s="103"/>
+      <c r="V54" s="103"/>
+      <c r="W54" s="103"/>
+      <c r="X54" s="103"/>
+      <c r="Y54" s="103"/>
+      <c r="Z54" s="103"/>
+      <c r="AA54" s="103"/>
+      <c r="AB54" s="103"/>
+      <c r="AC54" s="104"/>
+      <c r="AD54" s="105"/>
+      <c r="AE54" s="120"/>
+      <c r="AF54" s="106"/>
+      <c r="AG54" s="126"/>
+      <c r="AH54" s="127"/>
+      <c r="AI54" s="127"/>
+      <c r="AJ54" s="127"/>
+      <c r="AK54" s="127"/>
+      <c r="AL54" s="127"/>
+      <c r="AM54" s="127"/>
+      <c r="AN54" s="128"/>
     </row>
     <row r="55" spans="1:60" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="171"/>
-      <c r="B55" s="190">
+      <c r="A55" s="120"/>
+      <c r="B55" s="156">
         <v>51</v>
       </c>
-      <c r="C55" s="191"/>
-      <c r="D55" s="196" t="s">
+      <c r="C55" s="157"/>
+      <c r="D55" s="101" t="s">
         <v>8</v>
       </c>
-      <c r="E55" s="197"/>
-      <c r="F55" s="198"/>
-      <c r="G55" s="198"/>
-      <c r="H55" s="198"/>
-      <c r="I55" s="198"/>
-      <c r="J55" s="198"/>
-      <c r="K55" s="198"/>
-      <c r="L55" s="198"/>
-      <c r="M55" s="198"/>
-      <c r="N55" s="198"/>
-      <c r="O55" s="198"/>
-      <c r="P55" s="198"/>
-      <c r="Q55" s="198"/>
-      <c r="R55" s="198"/>
-      <c r="S55" s="198"/>
-      <c r="T55" s="198"/>
-      <c r="U55" s="198"/>
-      <c r="V55" s="198"/>
-      <c r="W55" s="198"/>
-      <c r="X55" s="198"/>
-      <c r="Y55" s="198"/>
-      <c r="Z55" s="198"/>
-      <c r="AA55" s="198"/>
-      <c r="AB55" s="198"/>
-      <c r="AC55" s="199"/>
-      <c r="AD55" s="200"/>
-      <c r="AE55" s="171"/>
-      <c r="AF55" s="201">
+      <c r="E55" s="102"/>
+      <c r="F55" s="103"/>
+      <c r="G55" s="103"/>
+      <c r="H55" s="103"/>
+      <c r="I55" s="103"/>
+      <c r="J55" s="103"/>
+      <c r="K55" s="103"/>
+      <c r="L55" s="103"/>
+      <c r="M55" s="103"/>
+      <c r="N55" s="103"/>
+      <c r="O55" s="103"/>
+      <c r="P55" s="103"/>
+      <c r="Q55" s="103"/>
+      <c r="R55" s="103"/>
+      <c r="S55" s="103"/>
+      <c r="T55" s="103"/>
+      <c r="U55" s="103"/>
+      <c r="V55" s="103"/>
+      <c r="W55" s="103"/>
+      <c r="X55" s="103"/>
+      <c r="Y55" s="103"/>
+      <c r="Z55" s="103"/>
+      <c r="AA55" s="103"/>
+      <c r="AB55" s="103"/>
+      <c r="AC55" s="104"/>
+      <c r="AD55" s="105"/>
+      <c r="AE55" s="120"/>
+      <c r="AF55" s="106">
         <v>37</v>
       </c>
-      <c r="AG55" s="203" t="s">
+      <c r="AG55" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="AH55" s="204"/>
-      <c r="AI55" s="204"/>
-      <c r="AJ55" s="204"/>
-      <c r="AK55" s="204"/>
-      <c r="AL55" s="204"/>
-      <c r="AM55" s="204"/>
-      <c r="AN55" s="205"/>
+      <c r="AH55" s="109"/>
+      <c r="AI55" s="109"/>
+      <c r="AJ55" s="109"/>
+      <c r="AK55" s="109"/>
+      <c r="AL55" s="109"/>
+      <c r="AM55" s="109"/>
+      <c r="AN55" s="110"/>
     </row>
     <row r="56" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="172"/>
-      <c r="B56" s="192">
+      <c r="A56" s="121"/>
+      <c r="B56" s="158">
         <v>52</v>
       </c>
-      <c r="C56" s="193"/>
-      <c r="D56" s="209" t="s">
+      <c r="C56" s="159"/>
+      <c r="D56" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E56" s="210"/>
-      <c r="F56" s="211"/>
-      <c r="G56" s="211"/>
-      <c r="H56" s="211"/>
-      <c r="I56" s="211"/>
-      <c r="J56" s="211"/>
-      <c r="K56" s="211"/>
-      <c r="L56" s="211"/>
-      <c r="M56" s="211"/>
-      <c r="N56" s="211"/>
-      <c r="O56" s="211"/>
-      <c r="P56" s="211"/>
-      <c r="Q56" s="211"/>
-      <c r="R56" s="211"/>
-      <c r="S56" s="211"/>
-      <c r="T56" s="211"/>
-      <c r="U56" s="211"/>
-      <c r="V56" s="211"/>
-      <c r="W56" s="211"/>
-      <c r="X56" s="211"/>
-      <c r="Y56" s="211"/>
-      <c r="Z56" s="211"/>
-      <c r="AA56" s="211"/>
-      <c r="AB56" s="211"/>
-      <c r="AC56" s="212"/>
-      <c r="AD56" s="213"/>
-      <c r="AE56" s="172"/>
-      <c r="AF56" s="202"/>
-      <c r="AG56" s="206"/>
-      <c r="AH56" s="207"/>
-      <c r="AI56" s="207"/>
-      <c r="AJ56" s="207"/>
-      <c r="AK56" s="207"/>
-      <c r="AL56" s="207"/>
-      <c r="AM56" s="207"/>
-      <c r="AN56" s="208"/>
+      <c r="E56" s="115"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="116"/>
+      <c r="H56" s="116"/>
+      <c r="I56" s="116"/>
+      <c r="J56" s="116"/>
+      <c r="K56" s="116"/>
+      <c r="L56" s="116"/>
+      <c r="M56" s="116"/>
+      <c r="N56" s="116"/>
+      <c r="O56" s="116"/>
+      <c r="P56" s="116"/>
+      <c r="Q56" s="116"/>
+      <c r="R56" s="116"/>
+      <c r="S56" s="116"/>
+      <c r="T56" s="116"/>
+      <c r="U56" s="116"/>
+      <c r="V56" s="116"/>
+      <c r="W56" s="116"/>
+      <c r="X56" s="116"/>
+      <c r="Y56" s="116"/>
+      <c r="Z56" s="116"/>
+      <c r="AA56" s="116"/>
+      <c r="AB56" s="116"/>
+      <c r="AC56" s="117"/>
+      <c r="AD56" s="118"/>
+      <c r="AE56" s="121"/>
+      <c r="AF56" s="107"/>
+      <c r="AG56" s="111"/>
+      <c r="AH56" s="112"/>
+      <c r="AI56" s="112"/>
+      <c r="AJ56" s="112"/>
+      <c r="AK56" s="112"/>
+      <c r="AL56" s="112"/>
+      <c r="AM56" s="112"/>
+      <c r="AN56" s="113"/>
     </row>
   </sheetData>
   <sheetProtection password="84CA" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="200">
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="AC5:AN9"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="X9:AA9"/>
+    <mergeCell ref="AC1:AN4"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="M2:T2"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="X4:AA4"/>
+    <mergeCell ref="F4:L4"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="F6:L6"/>
+    <mergeCell ref="A1:E9"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="M1:T1"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="F8:L8"/>
+    <mergeCell ref="F9:L9"/>
+    <mergeCell ref="M9:T9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="S37:T37"/>
+    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="U38:W38"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="U27:W27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U34:W34"/>
+    <mergeCell ref="AN11:AN12"/>
+    <mergeCell ref="A13:A41"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="AH11:AH12"/>
+    <mergeCell ref="AI11:AI12"/>
+    <mergeCell ref="AJ11:AJ12"/>
+    <mergeCell ref="AK11:AK12"/>
+    <mergeCell ref="AL11:AL12"/>
+    <mergeCell ref="AM11:AM12"/>
+    <mergeCell ref="AB11:AB12"/>
+    <mergeCell ref="AC11:AC12"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="S11:T12"/>
+    <mergeCell ref="U11:W12"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="AF11:AF12"/>
+    <mergeCell ref="AG11:AG12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="S30:T30"/>
+    <mergeCell ref="U30:W30"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="S36:T36"/>
+    <mergeCell ref="U36:W36"/>
+    <mergeCell ref="U35:W35"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="U42:W42"/>
+    <mergeCell ref="U41:W41"/>
+    <mergeCell ref="A49:A56"/>
+    <mergeCell ref="D49:AD49"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="U48:W48"/>
+    <mergeCell ref="A43:E47"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="S43:T43"/>
+    <mergeCell ref="U43:W43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="U44:W44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="S46:T46"/>
+    <mergeCell ref="U46:W46"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="D55:AD55"/>
+    <mergeCell ref="AF55:AF56"/>
+    <mergeCell ref="AG55:AN56"/>
+    <mergeCell ref="D56:AD56"/>
+    <mergeCell ref="AE49:AE56"/>
+    <mergeCell ref="AF49:AF50"/>
+    <mergeCell ref="AG49:AN50"/>
+    <mergeCell ref="D50:AD50"/>
+    <mergeCell ref="D51:AD51"/>
+    <mergeCell ref="AF51:AF52"/>
+    <mergeCell ref="AG51:AN52"/>
+    <mergeCell ref="D52:AD52"/>
+    <mergeCell ref="D53:AD53"/>
+    <mergeCell ref="AF53:AF54"/>
+    <mergeCell ref="AG53:AN54"/>
+    <mergeCell ref="D54:AD54"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="S47:T47"/>
+    <mergeCell ref="U47:W47"/>
+    <mergeCell ref="M42:N42"/>
     <mergeCell ref="N5:O6"/>
     <mergeCell ref="P5:Q6"/>
     <mergeCell ref="R5:S6"/>
@@ -5522,182 +5699,6 @@
     <mergeCell ref="M40:N40"/>
     <mergeCell ref="S40:T40"/>
     <mergeCell ref="U40:W40"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="S41:T41"/>
-    <mergeCell ref="D55:AD55"/>
-    <mergeCell ref="AF55:AF56"/>
-    <mergeCell ref="AG55:AN56"/>
-    <mergeCell ref="D56:AD56"/>
-    <mergeCell ref="AE49:AE56"/>
-    <mergeCell ref="AF49:AF50"/>
-    <mergeCell ref="AG49:AN50"/>
-    <mergeCell ref="D50:AD50"/>
-    <mergeCell ref="D51:AD51"/>
-    <mergeCell ref="AF51:AF52"/>
-    <mergeCell ref="AG51:AN52"/>
-    <mergeCell ref="D52:AD52"/>
-    <mergeCell ref="D53:AD53"/>
-    <mergeCell ref="AF53:AF54"/>
-    <mergeCell ref="AG53:AN54"/>
-    <mergeCell ref="D54:AD54"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="S47:T47"/>
-    <mergeCell ref="U47:W47"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="U42:W42"/>
-    <mergeCell ref="U41:W41"/>
-    <mergeCell ref="A49:A56"/>
-    <mergeCell ref="D49:AD49"/>
-    <mergeCell ref="M48:N48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="U48:W48"/>
-    <mergeCell ref="A43:E47"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="S43:T43"/>
-    <mergeCell ref="U43:W43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="U44:W44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="S46:T46"/>
-    <mergeCell ref="U46:W46"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="AE11:AE12"/>
-    <mergeCell ref="AF11:AF12"/>
-    <mergeCell ref="AG11:AG12"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="S30:T30"/>
-    <mergeCell ref="U30:W30"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="S36:T36"/>
-    <mergeCell ref="U36:W36"/>
-    <mergeCell ref="U35:W35"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="AN11:AN12"/>
-    <mergeCell ref="A13:A41"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="S13:T13"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="AH11:AH12"/>
-    <mergeCell ref="AI11:AI12"/>
-    <mergeCell ref="AJ11:AJ12"/>
-    <mergeCell ref="AK11:AK12"/>
-    <mergeCell ref="AL11:AL12"/>
-    <mergeCell ref="AM11:AM12"/>
-    <mergeCell ref="AB11:AB12"/>
-    <mergeCell ref="AC11:AC12"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="S16:T16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="S11:T12"/>
-    <mergeCell ref="U11:W12"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="S37:T37"/>
-    <mergeCell ref="U37:W37"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="U38:W38"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="U27:W27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="S17:T17"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="U18:W18"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="F6:L6"/>
-    <mergeCell ref="A1:E9"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="M1:T1"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="F8:L8"/>
-    <mergeCell ref="F9:L9"/>
-    <mergeCell ref="M9:T9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="AC1:AN4"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="M2:T2"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="X4:AA4"/>
-    <mergeCell ref="F4:L4"/>
-    <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U34:W34"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="AC5:AN9"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="X9:AA9"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="U23:W23"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.6692913385826772" bottom="0.36" header="0.31496062992125984" footer="0.24"/>

</xml_diff>

<commit_message>
Atualizado IEI, desativado IEE
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IEI.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IEI.XLSX
@@ -115,154 +115,154 @@
     <t>IEI</t>
   </si>
   <si>
+    <t>ROBERTO F.DO NASCIMENTO</t>
+  </si>
+  <si>
+    <t>1878</t>
+  </si>
+  <si>
     <t>ROBERTO CARLOS DINIZ</t>
   </si>
   <si>
     <t>2045</t>
   </si>
   <si>
+    <t>2612</t>
+  </si>
+  <si>
+    <t>3058</t>
+  </si>
+  <si>
+    <t>3257</t>
+  </si>
+  <si>
+    <t>3315</t>
+  </si>
+  <si>
+    <t>3385</t>
+  </si>
+  <si>
+    <t>3458</t>
+  </si>
+  <si>
+    <t>3492</t>
+  </si>
+  <si>
+    <t>3596</t>
+  </si>
+  <si>
+    <t>3599</t>
+  </si>
+  <si>
+    <t>3946</t>
+  </si>
+  <si>
+    <t>3947</t>
+  </si>
+  <si>
+    <t>3948</t>
+  </si>
+  <si>
+    <t>3949</t>
+  </si>
+  <si>
+    <t>3950</t>
+  </si>
+  <si>
+    <t>3984</t>
+  </si>
+  <si>
+    <t>4020</t>
+  </si>
+  <si>
+    <t>4232</t>
+  </si>
+  <si>
+    <t>4262</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>SIVAMILTON AYOLPHI</t>
+  </si>
+  <si>
     <t>JOSE MARCIO DA SILVA JUNIOR</t>
   </si>
   <si>
-    <t>3058</t>
-  </si>
-  <si>
-    <t>3349</t>
-  </si>
-  <si>
-    <t>3437</t>
-  </si>
-  <si>
-    <t>3458</t>
-  </si>
-  <si>
-    <t>3946</t>
-  </si>
-  <si>
-    <t>3949</t>
-  </si>
-  <si>
-    <t>3950</t>
-  </si>
-  <si>
-    <t>4020</t>
-  </si>
-  <si>
-    <t>4232</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>ELISA DO NASCIMENTO NUNES</t>
-  </si>
-  <si>
-    <t>GABRIEL JOSE DA SILVA E SILVA</t>
+    <t>MONA LISA ARRUDA</t>
+  </si>
+  <si>
+    <t>LUZIA VASCONCELOS G DA SILVA</t>
+  </si>
+  <si>
+    <t>JOSE VAGNER DA SILVA ALVES</t>
   </si>
   <si>
     <t>GERSON RONELLI F CARNEIRO</t>
   </si>
   <si>
+    <t>CEIR FERNANDES DE SOUZA FILHO</t>
+  </si>
+  <si>
+    <t>RODRIGO LEANDRO C. DANQUIMAIA</t>
+  </si>
+  <si>
+    <t>SWELLEN NATASHA P. BARBOSA DE SIQUEIRA</t>
+  </si>
+  <si>
     <t>VICTOR DE LYRA</t>
   </si>
   <si>
+    <t>MARCELO BITENCOURT</t>
+  </si>
+  <si>
+    <t>RENATO DA SILVA MONCORES</t>
+  </si>
+  <si>
     <t>ARI DE OLIVEIRA SANTOS JUNIOR</t>
   </si>
   <si>
     <t>LUIZ CARLOS CHAVES DE OLIVEIRA</t>
   </si>
   <si>
+    <t>VINICIUS FARJADO LIMA</t>
+  </si>
+  <si>
     <t>HEVERTTON NILDO M DO ROSARIO</t>
   </si>
   <si>
     <t>ARTUR LUCIO DUARTE NETO</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
+    <t>GABRIEL CAMARGO BATISTA*</t>
   </si>
   <si>
     <t> </t>

</xml_diff>